<commit_message>
further comment of print
</commit_message>
<xml_diff>
--- a/analysis/latest/terms.xlsx
+++ b/analysis/latest/terms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimd999/research/script_not_in_dropbox/srpAnalytics/analysis/latest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAF307E-1AE1-574E-9D2D-E8F0F35ED10C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4446534-D3F1-524E-AFEE-9762A60DB3AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15960" windowHeight="14600" xr2:uid="{F882FDEF-851F-DC4A-B978-FE9B8FD86AFC}"/>
+    <workbookView xWindow="28920" yWindow="9900" windowWidth="15960" windowHeight="14600" xr2:uid="{F882FDEF-851F-DC4A-B978-FE9B8FD86AFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update for phase III
</commit_message>
<xml_diff>
--- a/analysis/latest/terms.xlsx
+++ b/analysis/latest/terms.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimd999/research/script_not_in_dropbox/srpAnalytics/analysis/latest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4446534-D3F1-524E-AFEE-9762A60DB3AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EE3145-F358-0142-A873-BD69E7A19A4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28920" yWindow="9900" windowWidth="15960" windowHeight="14600" xr2:uid="{F882FDEF-851F-DC4A-B978-FE9B8FD86AFC}"/>
+    <workbookView xWindow="6660" yWindow="15020" windowWidth="20100" windowHeight="11680" xr2:uid="{F882FDEF-851F-DC4A-B978-FE9B8FD86AFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$29</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t>term</t>
   </si>
@@ -181,16 +181,101 @@
   </si>
   <si>
     <t>they are larvae now, essentially small fish and can swim around</t>
+  </si>
+  <si>
+    <t>DataQC_Flag</t>
+  </si>
+  <si>
+    <t>bmd_analysis_flag</t>
+  </si>
+  <si>
+    <t>BMD10_Flag</t>
+  </si>
+  <si>
+    <t>Not enough dose groups for BMD analysis. BMD analysis not performed.</t>
+  </si>
+  <si>
+    <t>No trend detected in dose-response data. BMD analysis not performed.</t>
+  </si>
+  <si>
+    <t>Dose-response data quality very good.</t>
+  </si>
+  <si>
+    <t>Dose-response data quality good.</t>
+  </si>
+  <si>
+    <t>Data resolution poor. Caution advised.</t>
+  </si>
+  <si>
+    <t>Negative correlation detected in dose-response data. Caution advised.</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>no model is selected in the first place</t>
+  </si>
+  <si>
+    <t>Convergence not achieved for any dose-response model.</t>
+  </si>
+  <si>
+    <t>Model fit might be unreliable. p-val for chi-squared statistic was &lt; 0.1 for all converged models.</t>
+  </si>
+  <si>
+    <t>A unique model could not be determined. Multiple models had the same AIC and BMD values but no valid BMDL values.</t>
+  </si>
+  <si>
+    <t>Multiple models found. User advised to look at the results of analysis to choose the best model.</t>
+  </si>
+  <si>
+    <t>BMD10 &lt; lowest_test_dose</t>
+  </si>
+  <si>
+    <t>BMD10 &gt; Highest_test_dose</t>
+  </si>
+  <si>
+    <t>lowest_test_dose &lt; BMD10 &lt; Highest_test_dose</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -216,8 +301,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,199 +635,333 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6628B642-8DBE-B143-BB83-8906A12E6441}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.33203125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2">
+        <v>5</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="5">
+        <v>-1</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5">
+        <v>1</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5">
+        <v>0</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C24" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D25" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C26" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C27" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C28" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B29" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D15" xr:uid="{653FA9A4-0C92-5449-9984-ED304975102D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D15">
-      <sortCondition ref="A1:A15"/>
+  <autoFilter ref="A1:D29" xr:uid="{653FA9A4-0C92-5449-9984-ED304975102D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D29">
+      <sortCondition ref="A1:A29"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated that LPR, morpho work
</commit_message>
<xml_diff>
--- a/analysis/latest/terms.xlsx
+++ b/analysis/latest/terms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimd999/research/script_not_in_dropbox/srpAnalytics/analysis/latest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97B70E5-B285-EB49-A542-B92B6873275B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984DC44B-E531-D644-B63E-7FCD5DCBB168}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6000" yWindow="500" windowWidth="21220" windowHeight="17460" xr2:uid="{F882FDEF-851F-DC4A-B978-FE9B8FD86AFC}"/>
   </bookViews>
@@ -658,7 +658,7 @@
       <pane xSplit="3" ySplit="10" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomRight" activeCell="C26" sqref="A25:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>